<commit_message>
Update docs on batteries.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-batteries-LiO2.xlsx
+++ b/premise/data/additional_inventories/lci-batteries-LiO2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67E30E1-E1F3-D040-82E5-3707D3E1CBCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8154B7B2-593D-A24A-A242-B2014310BA7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32880" yWindow="320" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Battery - LiO2" sheetId="1" r:id="rId1"/>
@@ -1265,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T541"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A277" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A300" sqref="A300"/>
+    <sheetView tabSelected="1" topLeftCell="A261" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H295" sqref="H295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5494,8 +5494,8 @@
         <v>27</v>
       </c>
       <c r="G296" t="str">
-        <f>B291</f>
-        <v>kilogram</v>
+        <f>B290</f>
+        <v>battery, Li-O2</v>
       </c>
     </row>
     <row r="297" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix missing units for external scenarios during datapackage export Fix LCIs that were picked up by validation.py
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-batteries-LiO2.xlsx
+++ b/premise/data/additional_inventories/lci-batteries-LiO2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10817"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1B0080-1DCB-DF4F-A03B-09A6B5AC1CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A44D40-4903-1D46-8935-660A807501ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38240" yWindow="-600" windowWidth="25800" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Battery - LiO2" sheetId="1" r:id="rId1"/>
@@ -1268,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T541"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A261" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B288" sqref="B288"/>
+    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A164" sqref="A164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3507,8 +3507,8 @@
         <v>118</v>
       </c>
       <c r="B164">
-        <f>0.234</f>
-        <v>0.23400000000000001</v>
+        <f>0.234*-1</f>
+        <v>-0.23400000000000001</v>
       </c>
       <c r="C164" t="s">
         <v>9</v>
@@ -3524,7 +3524,7 @@
       </c>
       <c r="H164">
         <f t="shared" si="0"/>
-        <v>2.4541919999999999</v>
+        <v>-2.4541919999999999</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
@@ -7129,7 +7129,8 @@
         <v>118</v>
       </c>
       <c r="B405" s="3">
-        <v>4.1000000000000002E-2</v>
+        <f>0.041*-1</f>
+        <v>-4.1000000000000002E-2</v>
       </c>
       <c r="C405" t="s">
         <v>9</v>

</xml_diff>